<commit_message>
added test cases for n - 1 and n in excel
</commit_message>
<xml_diff>
--- a/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab3/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD32F96-BB3D-4BEC-84C2-F065360E0972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19A6CED-233D-4373-A183-25312824391A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="129">
   <si>
     <t>Informaţiile vor fi preluate din fişiere text.</t>
   </si>
@@ -549,13 +549,83 @@
     <t>F02_Condn7 !isRepeated() &amp;&amp; current.before(time) &amp;&amp; isActive()</t>
   </si>
   <si>
-    <t>i &lt;= end.getTime()</t>
-  </si>
-  <si>
     <t>Vaida Radu Andrei</t>
   </si>
   <si>
     <t>Sofran Daniel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">F02. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Afisarea task-rilor planificate intr-o anumita perioada de timp, precizata ca data si ora de inceput si
+data si ora de sfarsit.</t>
+    </r>
+  </si>
+  <si>
+    <t>F02_TC00</t>
+  </si>
+  <si>
+    <t>null pointer exception</t>
+  </si>
+  <si>
+    <t>NullPointerException</t>
+  </si>
+  <si>
+    <t>F02_P00</t>
+  </si>
+  <si>
+    <t>99 - 100€</t>
+  </si>
+  <si>
+    <t>99 - 100 - 101 - 102 - 103 - 104 - 107 - 108-  109 - 110 - 111 - 112 - 108 - 109</t>
+  </si>
+  <si>
+    <t>99 - 100 - 101 - 102 - 103 - 104 - 107- 10 -  109 - 110 - 111 - 112 - 108 - 109</t>
+  </si>
+  <si>
+    <t>n-1</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>m &lt; n</t>
+  </si>
+  <si>
+    <t>n+1</t>
+  </si>
+  <si>
+    <t>F02_TC07</t>
+  </si>
+  <si>
+    <t>F02_TC08</t>
+  </si>
+  <si>
+    <t>"2023-02-22 09:59"</t>
+  </si>
+  <si>
+    <t>"2023-02-22 09:48"</t>
+  </si>
+  <si>
+    <t>"Wed Feb 22 09:48:12 EET 2023"</t>
+  </si>
+  <si>
+    <t>"Wed Feb 22 09:59:12 EET 2023"</t>
   </si>
 </sst>
 </file>
@@ -777,7 +847,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1236,11 +1306,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1279,9 +1371,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1321,6 +1410,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1333,6 +1425,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1342,9 +1440,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1372,18 +1467,33 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1393,23 +1503,77 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1441,9 +1605,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1459,73 +1620,55 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1550,15 +1693,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>567690</xdr:colOff>
+      <xdr:colOff>559223</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>93980</xdr:rowOff>
+      <xdr:rowOff>51647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>8467</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>126396</xdr:rowOff>
+      <xdr:rowOff>84063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1581,7 +1724,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="567690" y="1211580"/>
+          <a:off x="559223" y="1169247"/>
           <a:ext cx="8660977" cy="4130283"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1937,7 +2080,7 @@
   <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1955,7 +2098,7 @@
       <c r="G1" s="40"/>
     </row>
     <row r="2" spans="2:16">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1973,21 +2116,21 @@
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23" t="s">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1996,13 +2139,13 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="O7" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" s="23">
+      <c r="O7" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="P7" s="22">
         <v>237</v>
       </c>
     </row>
@@ -2011,13 +2154,13 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="P8" s="23">
+      <c r="O8" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="P8" s="22">
         <v>237</v>
       </c>
     </row>
@@ -2028,11 +2171,11 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="22"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" t="s">
@@ -2043,7 +2186,7 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="1"/>
@@ -2077,8 +2220,8 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2102,18 +2245,18 @@
       <c r="I1" s="40"/>
     </row>
     <row r="3" spans="2:20">
-      <c r="B3" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="44"/>
+      <c r="B3" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="38" t="s">
@@ -2122,8 +2265,8 @@
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="40"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="I6" s="38" t="s">
         <v>45</v>
       </c>
@@ -2141,7 +2284,7 @@
       <c r="T6" s="39"/>
     </row>
     <row r="8" spans="2:20">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="56" t="s">
@@ -2149,126 +2292,126 @@
       </c>
       <c r="D8" s="56"/>
       <c r="E8" s="56"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
       <c r="I8" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="Q8" s="55" t="s">
+      <c r="Q8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="55"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="30">
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="29">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:20">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="I9" s="34"/>
-      <c r="Q9" s="55" t="s">
+      <c r="C9" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="I9" s="33"/>
+      <c r="Q9" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="R9" s="55"/>
-      <c r="S9" s="55"/>
-      <c r="T9" s="30">
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="29">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:20">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="48"/>
-      <c r="Q10" s="55" t="s">
+      <c r="C10" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="49"/>
+      <c r="Q10" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="55" t="s">
+      <c r="R10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="55"/>
-      <c r="T10" s="30">
-        <v>16</v>
+      <c r="S10" s="43"/>
+      <c r="T10" s="29">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:20">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="51"/>
+      <c r="C11" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="52"/>
     </row>
     <row r="12" spans="2:20">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
+      <c r="C12" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
     </row>
     <row r="13" spans="2:20">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
+      <c r="C13" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
+      <c r="N13" s="51"/>
+      <c r="O13" s="52"/>
       <c r="Q13" s="38" t="s">
         <v>47</v>
       </c>
@@ -2277,33 +2420,33 @@
       <c r="T13" s="39"/>
     </row>
     <row r="14" spans="2:20">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="51"/>
+      <c r="C14" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="52"/>
     </row>
     <row r="15" spans="2:20">
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="51"/>
-      <c r="Q15" s="28" t="s">
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="52"/>
+      <c r="Q15" s="27" t="s">
         <v>15</v>
       </c>
       <c r="R15" s="56" t="s">
@@ -2313,147 +2456,145 @@
       <c r="T15" s="56"/>
     </row>
     <row r="16" spans="2:20">
-      <c r="I16" s="49"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="51"/>
-      <c r="Q16" s="31" t="s">
-        <v>50</v>
+      <c r="I16" s="50"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
+      <c r="N16" s="51"/>
+      <c r="O16" s="52"/>
+      <c r="Q16" s="30" t="s">
+        <v>115</v>
       </c>
       <c r="R16" s="41" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
       <c r="S16" s="41"/>
       <c r="T16" s="41"/>
     </row>
     <row r="17" spans="9:20">
-      <c r="I17" s="49"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="51"/>
-      <c r="Q17" s="31" t="s">
-        <v>51</v>
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="52"/>
+      <c r="Q17" s="30" t="s">
+        <v>50</v>
       </c>
       <c r="R17" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S17" s="41"/>
       <c r="T17" s="41"/>
     </row>
     <row r="18" spans="9:20">
-      <c r="I18" s="49"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="51"/>
-      <c r="Q18" s="31" t="s">
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
+      <c r="N18" s="51"/>
+      <c r="O18" s="52"/>
+      <c r="Q18" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+    </row>
+    <row r="19" spans="9:20">
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="52"/>
+      <c r="Q19" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="R18" s="41" t="s">
+      <c r="R19" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-    </row>
-    <row r="19" spans="9:20">
-      <c r="I19" s="49"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="51"/>
-      <c r="Q19" s="31" t="s">
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+    </row>
+    <row r="20" spans="9:20">
+      <c r="I20" s="50"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="52"/>
+      <c r="Q20" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="R19" s="41" t="s">
+      <c r="R20" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-    </row>
-    <row r="20" spans="9:20">
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="51"/>
-      <c r="Q20" s="31" t="s">
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+    </row>
+    <row r="21" spans="9:20">
+      <c r="I21" s="50"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="52"/>
+      <c r="Q21" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="41" t="s">
+      <c r="R21" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-    </row>
-    <row r="21" spans="9:20">
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="51"/>
-      <c r="Q21" s="31" t="s">
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+    </row>
+    <row r="22" spans="9:20">
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="52"/>
+      <c r="Q22" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="R21" s="41" t="s">
+      <c r="R22" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
-    </row>
-    <row r="22" spans="9:20">
-      <c r="I22" s="49"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="51"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
     </row>
     <row r="23" spans="9:20">
-      <c r="I23" s="49"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="51"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="52"/>
     </row>
     <row r="24" spans="9:20">
-      <c r="I24" s="52"/>
-      <c r="J24" s="53"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="54"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="55"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
+  <mergeCells count="20">
     <mergeCell ref="D1:I1"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R21:T21"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="I10:O24"/>
@@ -2466,7 +2607,13 @@
     <mergeCell ref="I6:O6"/>
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2480,10 +2627,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:AF16"/>
+  <dimension ref="B1:AG18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -2504,16 +2651,16 @@
     <col min="19" max="19" width="11.77734375" customWidth="1"/>
     <col min="20" max="20" width="8.77734375" customWidth="1"/>
     <col min="21" max="21" width="8.88671875" customWidth="1"/>
-    <col min="25" max="25" width="9.109375" customWidth="1"/>
-    <col min="26" max="26" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="2.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="2.21875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" customWidth="1"/>
+    <col min="27" max="27" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="2.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32">
+    <row r="1" spans="2:33">
       <c r="B1" s="10"/>
       <c r="D1" s="38" t="s">
         <v>76</v>
@@ -2522,82 +2669,83 @@
       <c r="F1" s="39"/>
       <c r="G1" s="40"/>
     </row>
-    <row r="3" spans="2:32">
-      <c r="B3" s="42" t="s">
+    <row r="3" spans="2:33">
+      <c r="B3" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-    </row>
-    <row r="5" spans="2:32">
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+    </row>
+    <row r="5" spans="2:33">
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="2:32" ht="15.6">
-      <c r="B6" s="59" t="s">
+    <row r="6" spans="2:33" ht="15.6">
+      <c r="B6" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-      <c r="Z6" s="59"/>
-      <c r="AA6" s="59"/>
-      <c r="AB6" s="59"/>
-      <c r="AC6" s="59"/>
-      <c r="AD6" s="59"/>
-      <c r="AE6" s="59"/>
-      <c r="AF6" s="59"/>
-    </row>
-    <row r="7" spans="2:32" ht="15.6">
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="67" t="s">
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="65"/>
+      <c r="X6" s="65"/>
+      <c r="Y6" s="65"/>
+      <c r="Z6" s="65"/>
+      <c r="AA6" s="65"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="65"/>
+      <c r="AD6" s="65"/>
+      <c r="AE6" s="65"/>
+      <c r="AF6" s="65"/>
+      <c r="AG6" s="65"/>
+    </row>
+    <row r="7" spans="2:33" ht="15.6">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
       <c r="T7" s="63" t="s">
         <v>61</v>
       </c>
@@ -2606,53 +2754,54 @@
       <c r="W7" s="63"/>
       <c r="X7" s="63"/>
       <c r="Y7" s="63"/>
-      <c r="Z7" s="62" t="s">
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="AA7" s="62"/>
-      <c r="AB7" s="62"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="62"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="62"/>
-    </row>
-    <row r="8" spans="2:32" ht="15.6" customHeight="1">
-      <c r="B8" s="59"/>
-      <c r="C8" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="66" t="s">
+      <c r="AB7" s="64"/>
+      <c r="AC7" s="64"/>
+      <c r="AD7" s="64"/>
+      <c r="AE7" s="64"/>
+      <c r="AF7" s="64"/>
+      <c r="AG7" s="64"/>
+    </row>
+    <row r="8" spans="2:33" ht="15.6" customHeight="1">
+      <c r="B8" s="65"/>
+      <c r="C8" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66" t="s">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66" t="s">
+      <c r="I8" s="62"/>
+      <c r="J8" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="66"/>
-      <c r="L8" s="57" t="s">
+      <c r="K8" s="62"/>
+      <c r="L8" s="59" t="s">
         <v>103</v>
       </c>
-      <c r="M8" s="58"/>
-      <c r="N8" s="57" t="s">
+      <c r="M8" s="60"/>
+      <c r="N8" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57" t="s">
+      <c r="O8" s="60"/>
+      <c r="P8" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="57" t="s">
+      <c r="Q8" s="60"/>
+      <c r="R8" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="S8" s="58"/>
+      <c r="S8" s="60"/>
       <c r="T8" s="63" t="s">
         <v>50</v>
       </c>
@@ -2668,36 +2817,37 @@
       <c r="X8" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="Y8" s="63" t="s">
+      <c r="Y8" s="121"/>
+      <c r="Z8" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="Z8" s="62">
+      <c r="AA8" s="64">
         <v>0</v>
       </c>
-      <c r="AA8" s="62">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="62">
+      <c r="AB8" s="64">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="64">
         <v>2</v>
       </c>
-      <c r="AC8" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="62">
-        <v>5</v>
-      </c>
-      <c r="AE8" s="62">
-        <v>6</v>
-      </c>
-      <c r="AF8" s="62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="2:32" ht="15.6">
-      <c r="B9" s="59"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
+      <c r="AD8" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE8" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF8" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG8" s="64" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" ht="15.6">
+      <c r="B9" s="65"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="61"/>
       <c r="F9" s="11" t="s">
         <v>21</v>
       </c>
@@ -2745,32 +2895,31 @@
       <c r="V9" s="63"/>
       <c r="W9" s="63"/>
       <c r="X9" s="63"/>
-      <c r="Y9" s="63"/>
-      <c r="Z9" s="62"/>
-      <c r="AA9" s="62"/>
-      <c r="AB9" s="62"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="62"/>
-      <c r="AE9" s="62"/>
-      <c r="AF9" s="62"/>
-    </row>
-    <row r="10" spans="2:32" ht="18">
+      <c r="Y9" s="122"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="64"/>
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="64"/>
+      <c r="AF9" s="64"/>
+      <c r="AG9" s="64"/>
+    </row>
+    <row r="10" spans="2:33" ht="31.2">
       <c r="B10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>89</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" s="23">
-        <v>1</v>
-      </c>
-      <c r="G10" s="23"/>
+        <v>113</v>
+      </c>
+      <c r="E10" s="22">
+        <v>99</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
@@ -2783,41 +2932,42 @@
       <c r="Q10" s="14"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
-      <c r="T10" s="15"/>
+      <c r="T10" s="15">
+        <v>1</v>
+      </c>
       <c r="U10" s="15"/>
       <c r="V10" s="15"/>
       <c r="W10" s="15"/>
       <c r="X10" s="15"/>
       <c r="Y10" s="15"/>
-      <c r="Z10" s="16"/>
+      <c r="Z10" s="15"/>
       <c r="AA10" s="16"/>
       <c r="AB10" s="16"/>
       <c r="AC10" s="16"/>
       <c r="AD10" s="16"/>
       <c r="AE10" s="16"/>
       <c r="AF10" s="16"/>
-    </row>
-    <row r="11" spans="2:32" ht="18">
+      <c r="AG10" s="16"/>
+    </row>
+    <row r="11" spans="2:33" ht="18">
       <c r="B11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="35" t="s">
         <v>90</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23">
-        <v>1</v>
-      </c>
+      <c r="E11" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1</v>
+      </c>
+      <c r="G11" s="22"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
+      <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
@@ -2827,38 +2977,39 @@
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
       <c r="R11" s="14"/>
-      <c r="S11" s="14">
-        <v>1</v>
-      </c>
+      <c r="S11" s="14"/>
       <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
+      <c r="U11" s="15">
+        <v>1</v>
+      </c>
       <c r="V11" s="15"/>
       <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
-      <c r="Z11" s="16"/>
+      <c r="Z11" s="15"/>
       <c r="AA11" s="16"/>
       <c r="AB11" s="16"/>
       <c r="AC11" s="16"/>
       <c r="AD11" s="16"/>
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
-    </row>
-    <row r="12" spans="2:32" ht="18">
+      <c r="AG11" s="16"/>
+    </row>
+    <row r="12" spans="2:33" ht="18">
       <c r="B12" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23">
+        <v>49</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22">
         <v>1</v>
       </c>
       <c r="H12" s="14"/>
@@ -2873,48 +3024,49 @@
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
-      <c r="R12" s="14">
-        <v>1</v>
-      </c>
-      <c r="S12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14">
+        <v>1</v>
+      </c>
       <c r="T12" s="15"/>
       <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
+      <c r="V12" s="15">
+        <v>1</v>
+      </c>
       <c r="W12" s="15"/>
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
-      <c r="Z12" s="16"/>
+      <c r="Z12" s="15"/>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16"/>
       <c r="AC12" s="16"/>
       <c r="AD12" s="16"/>
       <c r="AE12" s="16"/>
       <c r="AF12" s="16"/>
-    </row>
-    <row r="13" spans="2:32" ht="18">
+      <c r="AG12" s="16"/>
+    </row>
+    <row r="13" spans="2:33" ht="18">
       <c r="B13" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23">
-        <v>1</v>
-      </c>
-      <c r="H13" s="14">
-        <v>1</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14">
-        <v>1</v>
-      </c>
+      <c r="E13" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14">
+        <v>1</v>
+      </c>
+      <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -2922,54 +3074,55 @@
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
+      <c r="R13" s="14">
+        <v>1</v>
+      </c>
       <c r="S13" s="14"/>
       <c r="T13" s="15"/>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
-      <c r="W13" s="15"/>
+      <c r="W13" s="15">
+        <v>1</v>
+      </c>
       <c r="X13" s="15"/>
       <c r="Y13" s="15"/>
-      <c r="Z13" s="16"/>
+      <c r="Z13" s="15"/>
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
       <c r="AC13" s="16"/>
       <c r="AD13" s="16"/>
       <c r="AE13" s="16"/>
       <c r="AF13" s="16"/>
-    </row>
-    <row r="14" spans="2:32" ht="18">
+      <c r="AG13" s="16"/>
+    </row>
+    <row r="14" spans="2:33" ht="18">
       <c r="B14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23">
+        <v>85</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22">
         <v>1</v>
       </c>
       <c r="H14" s="14">
         <v>1</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14">
-        <v>1</v>
-      </c>
-      <c r="L14" s="14">
-        <v>1</v>
-      </c>
+      <c r="J14" s="14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
       <c r="M14" s="14"/>
-      <c r="N14" s="14">
-        <v>1</v>
-      </c>
+      <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -2979,33 +3132,34 @@
       <c r="U14" s="15"/>
       <c r="V14" s="15"/>
       <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
+      <c r="X14" s="15">
+        <v>1</v>
+      </c>
       <c r="Y14" s="15"/>
-      <c r="Z14" s="16">
-        <v>1</v>
-      </c>
+      <c r="Z14" s="15"/>
       <c r="AA14" s="16"/>
       <c r="AB14" s="16"/>
       <c r="AC14" s="16"/>
       <c r="AD14" s="16"/>
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
-    </row>
-    <row r="15" spans="2:32" ht="18">
+      <c r="AG14" s="16"/>
+    </row>
+    <row r="15" spans="2:33" ht="18">
       <c r="B15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23">
+      <c r="E15" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22">
         <v>1</v>
       </c>
       <c r="H15" s="14">
@@ -3020,13 +3174,11 @@
         <v>1</v>
       </c>
       <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14">
-        <v>1</v>
-      </c>
-      <c r="P15" s="14">
-        <v>1</v>
-      </c>
+      <c r="N15" s="14">
+        <v>1</v>
+      </c>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
@@ -3035,38 +3187,225 @@
       <c r="V15" s="15"/>
       <c r="W15" s="15"/>
       <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="16">
-        <v>1</v>
-      </c>
+      <c r="Y15" s="15">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="15"/>
       <c r="AA15" s="16">
         <v>1</v>
       </c>
       <c r="AB15" s="16"/>
       <c r="AC15" s="16"/>
-      <c r="AD15" s="16">
-        <v>1</v>
-      </c>
+      <c r="AD15" s="16"/>
       <c r="AE15" s="16"/>
       <c r="AF15" s="16"/>
-    </row>
-    <row r="16" spans="2:32" ht="15.6">
-      <c r="B16" s="17"/>
+      <c r="AG15" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" ht="18">
+      <c r="B16" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14">
+        <v>1</v>
+      </c>
+      <c r="L16" s="14">
+        <v>1</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14">
+        <v>1</v>
+      </c>
+      <c r="P16" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>1</v>
+      </c>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="16"/>
+      <c r="AC16" s="16"/>
+      <c r="AD16" s="16"/>
+      <c r="AE16" s="16"/>
+      <c r="AF16" s="16"/>
+      <c r="AG16" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:33" ht="18">
+      <c r="B17" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22">
+        <v>1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14">
+        <v>1</v>
+      </c>
+      <c r="L17" s="14">
+        <v>1</v>
+      </c>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14">
+        <v>1</v>
+      </c>
+      <c r="P17" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>1</v>
+      </c>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
+      <c r="Z17" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="16"/>
+      <c r="AC17" s="16"/>
+      <c r="AD17" s="16">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="16"/>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="16"/>
+    </row>
+    <row r="18" spans="2:33" ht="18">
+      <c r="B18" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14">
+        <v>1</v>
+      </c>
+      <c r="L18" s="14">
+        <v>1</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14">
+        <v>1</v>
+      </c>
+      <c r="P18" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>1</v>
+      </c>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
+      <c r="Z18" s="15">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="16"/>
+      <c r="AD18" s="16"/>
+      <c r="AE18" s="16">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="16"/>
+      <c r="AG18" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:S7"/>
-    <mergeCell ref="T7:Y7"/>
+  <mergeCells count="33">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:AG6"/>
+    <mergeCell ref="AE8:AE9"/>
+    <mergeCell ref="AF8:AF9"/>
+    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="AB8:AB9"/>
     <mergeCell ref="AC8:AC9"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="AD8:AD9"/>
     <mergeCell ref="X8:X9"/>
-    <mergeCell ref="Z7:AF7"/>
-    <mergeCell ref="AF8:AF9"/>
+    <mergeCell ref="AA7:AG7"/>
+    <mergeCell ref="AG8:AG9"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="Z8:Z9"/>
+    <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:U9"/>
     <mergeCell ref="V8:V9"/>
@@ -3074,19 +3413,11 @@
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:AF6"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AE8:AE9"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:S7"/>
+    <mergeCell ref="T7:Z7"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3099,10 +3430,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:N17"/>
+  <dimension ref="B1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -3120,7 +3451,7 @@
     <col min="15" max="15" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="2:12">
       <c r="B1" s="10"/>
       <c r="D1" s="38" t="s">
         <v>76</v>
@@ -3129,145 +3460,119 @@
       <c r="F1" s="39"/>
       <c r="G1" s="40"/>
     </row>
-    <row r="3" spans="2:14">
-      <c r="B3" s="68" t="s">
+    <row r="3" spans="2:12">
+      <c r="B3" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="69" t="s">
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="77"/>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="71" t="s">
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="72"/>
-    </row>
-    <row r="5" spans="2:14" ht="15" thickBot="1">
-      <c r="B5" s="70"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="2" t="s">
+      <c r="L4" s="96"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="108"/>
+      <c r="C5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="113"/>
+    </row>
+    <row r="6" spans="2:12" ht="15" thickBot="1">
+      <c r="B6" s="94"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="98"/>
+      <c r="K6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="18.600000000000001" thickTop="1">
-      <c r="B6" s="18">
+    <row r="7" spans="2:12" ht="15" thickTop="1">
+      <c r="B7" s="114">
+        <v>8</v>
+      </c>
+      <c r="C7" s="115"/>
+      <c r="D7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="117" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="L7" s="120" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="18">
+      <c r="B8" s="17">
         <v>9</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C8" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E8" s="35" t="s">
         <v>90</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="83"/>
-      <c r="K6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="18">
-      <c r="B7" s="18">
-        <v>10</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="18">
-      <c r="B8" s="18">
-        <v>11</v>
-      </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>91</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>1</v>
@@ -3278,281 +3583,407 @@
       <c r="H8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="36" t="s">
+      <c r="I8" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="106"/>
+      <c r="K8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="18">
+      <c r="B9" s="17">
+        <v>10</v>
+      </c>
+      <c r="C9" s="99"/>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="96"/>
+      <c r="K9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="18">
+      <c r="B10" s="17">
+        <v>11</v>
+      </c>
+      <c r="C10" s="99"/>
+      <c r="D10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="96"/>
+      <c r="K10" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="36" t="s">
+      <c r="L10" s="35" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="18">
-      <c r="B9" s="18">
+    <row r="11" spans="2:12" ht="18">
+      <c r="B11" s="17">
         <v>11</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="4" t="s">
+      <c r="C11" s="99"/>
+      <c r="D11" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="18" t="s">
+      <c r="F11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="36" t="s">
+      <c r="H11" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="96"/>
+      <c r="K11" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="L9" s="36" t="s">
+      <c r="L11" s="35" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="18">
-      <c r="B10" s="18">
+    <row r="12" spans="2:12" ht="18">
+      <c r="B12" s="17">
         <v>12</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="4" t="s">
+      <c r="C12" s="99"/>
+      <c r="D12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="18" t="s">
+      <c r="F12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="72"/>
-      <c r="K10" s="36" t="s">
+      <c r="H12" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="96"/>
+      <c r="K12" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="36" t="s">
+      <c r="L12" s="35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="18.600000000000001" thickBot="1">
-      <c r="B11" s="2">
+    <row r="13" spans="2:12" ht="18.600000000000001" thickBot="1">
+      <c r="B13" s="2">
         <v>13</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="4" t="s">
+      <c r="C13" s="100"/>
+      <c r="D13" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E13" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="74"/>
-      <c r="K11" s="36" t="s">
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="98"/>
+      <c r="K13" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="L11" s="36" t="s">
+      <c r="L13" s="35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="18.600000000000001" thickTop="1">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:14" ht="15" thickBot="1">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="2:12" ht="19.2" thickTop="1" thickBot="1">
+      <c r="B14" s="2">
+        <v>14</v>
+      </c>
+      <c r="C14" s="123"/>
+      <c r="D14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="98"/>
+      <c r="K14" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="19.2" thickTop="1" thickBot="1">
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
+      <c r="C15" s="123"/>
+      <c r="D15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="98"/>
+      <c r="K15" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="18.600000000000001" thickTop="1">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:14" ht="15" thickBot="1">
+      <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
-      <c r="B14" s="86" t="s">
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="2:14" ht="15.6" thickTop="1" thickBot="1">
+      <c r="B18" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="105" t="s">
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="106"/>
-      <c r="H14" s="86" t="s">
+      <c r="G18" s="71"/>
+      <c r="H18" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="88"/>
-      <c r="M14" s="93" t="s">
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="N14" s="94"/>
-    </row>
-    <row r="15" spans="2:14" ht="15" thickTop="1">
-      <c r="B15" s="92" t="s">
+      <c r="N18" s="91"/>
+    </row>
+    <row r="19" spans="2:14" ht="15" thickTop="1">
+      <c r="B19" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C19" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="84" t="s">
+      <c r="D19" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E19" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F19" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="100" t="s">
+      <c r="G19" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="101" t="s">
+      <c r="H19" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="84" t="s">
+      <c r="I19" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="J15" s="84" t="s">
+      <c r="J19" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="103" t="s">
+      <c r="K19" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="89" t="s">
+      <c r="L19" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="M15" s="91" t="s">
+      <c r="M19" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="N15" s="78" t="s">
+      <c r="N19" s="73" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="95"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="97"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="85"/>
-      <c r="J16" s="85"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="92"/>
-      <c r="N16" s="98"/>
-    </row>
-    <row r="17" spans="2:14">
-      <c r="B17" s="23">
+    <row r="20" spans="2:14">
+      <c r="B20" s="82"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="88"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="74"/>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="22">
         <v>6</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C21" s="20">
         <v>6</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D21" s="20">
         <v>0</v>
       </c>
-      <c r="E17" s="37">
-        <v>1</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="8" t="s">
+      <c r="E21" s="36">
+        <v>1</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="I17" s="23">
-        <f>SUM(J17:K17)</f>
+      <c r="I21" s="22">
+        <f>SUM(J21:K21)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J21" s="20">
         <v>0</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K21" s="23">
         <v>0</v>
       </c>
-      <c r="L17" s="25"/>
-      <c r="M17" s="6" t="s">
+      <c r="L21" s="24"/>
+      <c r="M21" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="N17" s="26">
-        <f>C17</f>
+      <c r="N21" s="25">
+        <f>C21</f>
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="M14:N14"/>
+  <mergeCells count="34">
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="M18:N18"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I6:J6"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="C8:C13"/>
     <mergeCell ref="E4:J4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3561,6 +3992,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3704,22 +4150,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E53DB3A-2750-466D-B803-7A1FAB16D24B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3735,21 +4183,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>